<commit_message>
Added a new column populated
</commit_message>
<xml_diff>
--- a/PackageXML.xlsx
+++ b/PackageXML.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97353009-2867-41FD-ADED-D9E2D30DF977}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA6B324-1E7A-4E10-822D-5647A285804A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="931" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,7 +263,7 @@
     <sheet name="Sheet243" sheetId="244" r:id="rId253"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Metadata Types'!$A$2:$A$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Metadata Types'!$D$2:$D$127</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="181">
   <si>
     <t>Description/Comments</t>
   </si>
@@ -943,6 +943,9 @@
       <t xml:space="preserve">
 For the components residing in the public folder, enter the folder name as unfiled$public</t>
     </r>
+  </si>
+  <si>
+    <t>Populated</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1498,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,7 +2211,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,7 +2401,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2918,7 +2921,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5053,25 +5056,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A5A7B4-D271-4E83-B19E-4BDFE7A9A323}">
-  <dimension ref="A1:C127"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0"/>
+  <dimension ref="A1:D127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.42578125" customWidth="1"/>
     <col min="2" max="2" width="51.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
@@ -5081,8 +5088,11 @@
       <c r="C2" s="14" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -5091,7 +5101,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -5100,7 +5110,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5109,7 +5119,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -5121,7 +5131,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -5133,7 +5143,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -5142,7 +5152,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -5151,7 +5161,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5160,7 +5170,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -5169,7 +5179,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -5178,7 +5188,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -5187,7 +5197,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -5199,7 +5209,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -5208,7 +5218,7 @@
         <v>Click Here</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -6256,7 +6266,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:A127" xr:uid="{D7A2E98A-DD04-4283-912D-0441EA18B78A}"/>
+  <autoFilter ref="D2:D127" xr:uid="{CA0EB0F3-5ED0-4174-B87A-0099AFB00CB3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10682,7 +10692,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10945,7 +10955,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11396,7 +11406,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11844,7 +11854,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12110,7 +12120,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>